<commit_message>
have to check the rounding for cifar 10
</commit_message>
<xml_diff>
--- a/results/cifar10-on-ResNet18-add-gaussian-blur-gradient-based-attacks.xlsx
+++ b/results/cifar10-on-ResNet18-add-gaussian-blur-gradient-based-attacks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adzie\code\bandlimited-cnns\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0BFB9C7-30AD-4E24-976C-4EF8CC152045}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B0D6DF6-E373-4E48-9139-E2BDF811D76E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="18192" windowHeight="12192" tabRatio="807" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="18192" windowHeight="12192" tabRatio="807" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cifar10-on-ResNet18-add-gaussia" sheetId="1" r:id="rId1"/>
@@ -19,21 +19,14 @@
     <sheet name="results" sheetId="4" r:id="rId4"/>
     <sheet name="graphAdditiveUniformNoise" sheetId="5" r:id="rId5"/>
     <sheet name="GradientSignAttack" sheetId="6" r:id="rId6"/>
+    <sheet name="GradientSignRound" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="33">
   <si>
     <t>epsilon</t>
   </si>
@@ -126,6 +119,12 @@
   </si>
   <si>
     <t>counter:  1000  min:  -2.4290657  max:  2.7537313</t>
+  </si>
+  <si>
+    <t>attack type:  GradientSignAttack</t>
+  </si>
+  <si>
+    <t>GradientSignAttack</t>
   </si>
 </sst>
 </file>
@@ -5901,8 +5900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C9E714F-1323-4878-B5E9-E63B10F08A2E}">
   <dimension ref="A1:N71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView topLeftCell="H4" workbookViewId="0">
+      <selection activeCell="X10" sqref="X10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -7694,10 +7693,677 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A42:G53">
+  <sortState ref="A42:G53">
     <sortCondition ref="C42:C53"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20C460BE-E48D-4A66-A778-EE715080F31E}">
+  <dimension ref="A1:G32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="2" max="2" width="18.26171875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>96</v>
+      </c>
+      <c r="E3">
+        <v>100</v>
+      </c>
+      <c r="F3">
+        <v>0.96</v>
+      </c>
+      <c r="G3">
+        <v>156.348306894302</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4">
+        <v>1.0526315789473601E-2</v>
+      </c>
+      <c r="D4">
+        <v>58</v>
+      </c>
+      <c r="E4">
+        <v>100</v>
+      </c>
+      <c r="F4">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="G4">
+        <v>106.230905055999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5">
+        <v>2.1052631578947299E-2</v>
+      </c>
+      <c r="D5">
+        <v>54</v>
+      </c>
+      <c r="E5">
+        <v>100</v>
+      </c>
+      <c r="F5">
+        <v>0.54</v>
+      </c>
+      <c r="G5">
+        <v>101.094986200332</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6">
+        <v>3.1578947368420998E-2</v>
+      </c>
+      <c r="D6">
+        <v>52</v>
+      </c>
+      <c r="E6">
+        <v>100</v>
+      </c>
+      <c r="F6">
+        <v>0.52</v>
+      </c>
+      <c r="G6">
+        <v>98.363173484802203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7">
+        <v>4.2105263157894701E-2</v>
+      </c>
+      <c r="D7">
+        <v>48</v>
+      </c>
+      <c r="E7">
+        <v>100</v>
+      </c>
+      <c r="F7">
+        <v>0.48</v>
+      </c>
+      <c r="G7">
+        <v>93.032419443130493</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8">
+        <v>5.2631578947368397E-2</v>
+      </c>
+      <c r="D8">
+        <v>41</v>
+      </c>
+      <c r="E8">
+        <v>100</v>
+      </c>
+      <c r="F8">
+        <v>0.41</v>
+      </c>
+      <c r="G8">
+        <v>84.000523090362506</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9">
+        <v>6.3157894736842093E-2</v>
+      </c>
+      <c r="D9">
+        <v>35</v>
+      </c>
+      <c r="E9">
+        <v>100</v>
+      </c>
+      <c r="F9">
+        <v>0.35</v>
+      </c>
+      <c r="G9">
+        <v>76.381509065627995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10">
+        <v>7.3684210526315699E-2</v>
+      </c>
+      <c r="D10">
+        <v>31</v>
+      </c>
+      <c r="E10">
+        <v>100</v>
+      </c>
+      <c r="F10">
+        <v>0.31</v>
+      </c>
+      <c r="G10">
+        <v>70.736005783080998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>96</v>
+      </c>
+      <c r="E13">
+        <v>100</v>
+      </c>
+      <c r="F13">
+        <v>0.96</v>
+      </c>
+      <c r="G13">
+        <v>156.348306894302</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14">
+        <v>1.0526315789473601E-2</v>
+      </c>
+      <c r="D14">
+        <v>58</v>
+      </c>
+      <c r="E14">
+        <v>100</v>
+      </c>
+      <c r="F14">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="G14">
+        <v>106.230905055999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15">
+        <v>2.1052631578947299E-2</v>
+      </c>
+      <c r="D15">
+        <v>54</v>
+      </c>
+      <c r="E15">
+        <v>100</v>
+      </c>
+      <c r="F15">
+        <v>0.54</v>
+      </c>
+      <c r="G15">
+        <v>101.094986200332</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16">
+        <v>3.1578947368420998E-2</v>
+      </c>
+      <c r="D16">
+        <v>52</v>
+      </c>
+      <c r="E16">
+        <v>100</v>
+      </c>
+      <c r="F16">
+        <v>0.52</v>
+      </c>
+      <c r="G16">
+        <v>98.363173484802203</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17">
+        <v>4.2105263157894701E-2</v>
+      </c>
+      <c r="D17">
+        <v>48</v>
+      </c>
+      <c r="E17">
+        <v>100</v>
+      </c>
+      <c r="F17">
+        <v>0.48</v>
+      </c>
+      <c r="G17">
+        <v>93.032419443130493</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18">
+        <v>5.2631578947368397E-2</v>
+      </c>
+      <c r="D18">
+        <v>41</v>
+      </c>
+      <c r="E18">
+        <v>100</v>
+      </c>
+      <c r="F18">
+        <v>0.41</v>
+      </c>
+      <c r="G18">
+        <v>84.000523090362506</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19">
+        <v>0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19">
+        <v>6.3157894736842093E-2</v>
+      </c>
+      <c r="D19">
+        <v>35</v>
+      </c>
+      <c r="E19">
+        <v>100</v>
+      </c>
+      <c r="F19">
+        <v>0.35</v>
+      </c>
+      <c r="G19">
+        <v>76.381509065627995</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20">
+        <v>7.3684210526315699E-2</v>
+      </c>
+      <c r="D20">
+        <v>31</v>
+      </c>
+      <c r="E20">
+        <v>100</v>
+      </c>
+      <c r="F20">
+        <v>0.31</v>
+      </c>
+      <c r="G20">
+        <v>70.736005783080998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21">
+        <v>0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21">
+        <v>8.4210526315789402E-2</v>
+      </c>
+      <c r="D21">
+        <v>23</v>
+      </c>
+      <c r="E21">
+        <v>100</v>
+      </c>
+      <c r="F21">
+        <v>0.23</v>
+      </c>
+      <c r="G21">
+        <v>60.2207190990448</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22">
+        <v>9.4736842105263105E-2</v>
+      </c>
+      <c r="D22">
+        <v>19</v>
+      </c>
+      <c r="E22">
+        <v>100</v>
+      </c>
+      <c r="F22">
+        <v>0.19</v>
+      </c>
+      <c r="G22">
+        <v>54.863144874572697</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23">
+        <v>0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23">
+        <v>0.105263157894736</v>
+      </c>
+      <c r="D23">
+        <v>15</v>
+      </c>
+      <c r="E23">
+        <v>100</v>
+      </c>
+      <c r="F23">
+        <v>0.15</v>
+      </c>
+      <c r="G23">
+        <v>49.751561641693101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24">
+        <v>0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24">
+        <v>0.11578947368421</v>
+      </c>
+      <c r="D24">
+        <v>14</v>
+      </c>
+      <c r="E24">
+        <v>100</v>
+      </c>
+      <c r="F24">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G24">
+        <v>48.158949375152503</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25">
+        <v>0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25">
+        <v>0.12631578947368399</v>
+      </c>
+      <c r="D25">
+        <v>13</v>
+      </c>
+      <c r="E25">
+        <v>100</v>
+      </c>
+      <c r="F25">
+        <v>0.13</v>
+      </c>
+      <c r="G25">
+        <v>47.358682870864797</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26">
+        <v>0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26">
+        <v>0.13684210526315699</v>
+      </c>
+      <c r="D26">
+        <v>12</v>
+      </c>
+      <c r="E26">
+        <v>100</v>
+      </c>
+      <c r="F26">
+        <v>0.12</v>
+      </c>
+      <c r="G26">
+        <v>46.101258993148797</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27">
+        <v>0.14736842105263101</v>
+      </c>
+      <c r="D27">
+        <v>12</v>
+      </c>
+      <c r="E27">
+        <v>100</v>
+      </c>
+      <c r="F27">
+        <v>0.12</v>
+      </c>
+      <c r="G27">
+        <v>46.050325632095301</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28">
+        <v>0.157894736842105</v>
+      </c>
+      <c r="D28">
+        <v>12</v>
+      </c>
+      <c r="E28">
+        <v>100</v>
+      </c>
+      <c r="F28">
+        <v>0.12</v>
+      </c>
+      <c r="G28">
+        <v>46.863862037658599</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29">
+        <v>0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29">
+        <v>0.168421052631578</v>
+      </c>
+      <c r="D29">
+        <v>11</v>
+      </c>
+      <c r="E29">
+        <v>100</v>
+      </c>
+      <c r="F29">
+        <v>0.11</v>
+      </c>
+      <c r="G29">
+        <v>44.665889024734497</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30">
+        <v>0</v>
+      </c>
+      <c r="B30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30">
+        <v>0.17894736842105199</v>
+      </c>
+      <c r="D30">
+        <v>11</v>
+      </c>
+      <c r="E30">
+        <v>100</v>
+      </c>
+      <c r="F30">
+        <v>0.11</v>
+      </c>
+      <c r="G30">
+        <v>44.583665370941098</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31">
+        <v>0</v>
+      </c>
+      <c r="B31" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31">
+        <v>0.18947368421052599</v>
+      </c>
+      <c r="D31">
+        <v>11</v>
+      </c>
+      <c r="E31">
+        <v>100</v>
+      </c>
+      <c r="F31">
+        <v>0.11</v>
+      </c>
+      <c r="G31">
+        <v>44.622020244598303</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32">
+        <v>0</v>
+      </c>
+      <c r="B32" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32">
+        <v>0.2</v>
+      </c>
+      <c r="D32">
+        <v>8</v>
+      </c>
+      <c r="E32">
+        <v>100</v>
+      </c>
+      <c r="F32">
+        <v>0.08</v>
+      </c>
+      <c r="G32">
+        <v>40.623475313186603</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
how to do it for full cifar10
</commit_message>
<xml_diff>
--- a/results/cifar10-on-ResNet18-add-gaussian-blur-gradient-based-attacks.xlsx
+++ b/results/cifar10-on-ResNet18-add-gaussian-blur-gradient-based-attacks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adzie\code\bandlimited-cnns\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B0D6DF6-E373-4E48-9139-E2BDF811D76E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD75BD9-1233-4D06-B51E-047D20EBC5A2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="18192" windowHeight="12192" tabRatio="807" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="18192" windowHeight="12192" tabRatio="807" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cifar10-on-ResNet18-add-gaussia" sheetId="1" r:id="rId1"/>
@@ -20,13 +20,15 @@
     <sheet name="graphAdditiveUniformNoise" sheetId="5" r:id="rId5"/>
     <sheet name="GradientSignAttack" sheetId="6" r:id="rId6"/>
     <sheet name="GradientSignRound" sheetId="7" r:id="rId7"/>
+    <sheet name="spacing" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="37">
   <si>
     <t>epsilon</t>
   </si>
@@ -125,6 +127,18 @@
   </si>
   <si>
     <t>GradientSignAttack</t>
+  </si>
+  <si>
+    <t>dataset:  imagenet</t>
+  </si>
+  <si>
+    <t>spacing</t>
+  </si>
+  <si>
+    <t>dataset:  cifar10</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sum_difference</t>
   </si>
 </sst>
 </file>
@@ -7705,8 +7719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20C460BE-E48D-4A66-A778-EE715080F31E}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -8366,4 +8380,362 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D7BFA73-9793-4AD5-8067-A07AF1931C66}">
+  <dimension ref="A1:F21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>18</v>
+      </c>
+      <c r="C3">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <v>0.9</v>
+      </c>
+      <c r="E3">
+        <v>7.4878764152526802</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>17</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <v>0.85</v>
+      </c>
+      <c r="E4">
+        <v>1.8398396968841499</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>17</v>
+      </c>
+      <c r="C5">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <v>0.85</v>
+      </c>
+      <c r="E5">
+        <v>1.8233780860900799</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>17</v>
+      </c>
+      <c r="C6">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <v>0.85</v>
+      </c>
+      <c r="E6">
+        <v>1.83852338790893</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>16</v>
+      </c>
+      <c r="C7">
+        <v>20</v>
+      </c>
+      <c r="D7">
+        <v>0.8</v>
+      </c>
+      <c r="E7">
+        <v>1.9674994945526101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>32</v>
+      </c>
+      <c r="B8">
+        <v>13</v>
+      </c>
+      <c r="C8">
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <v>0.65</v>
+      </c>
+      <c r="E8">
+        <v>1.8854739665985101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <v>64</v>
+      </c>
+      <c r="B9">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>20</v>
+      </c>
+      <c r="D9">
+        <v>0.45</v>
+      </c>
+      <c r="E9">
+        <v>1.8965969085693299</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <v>128</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>20</v>
+      </c>
+      <c r="D10">
+        <v>0.1</v>
+      </c>
+      <c r="E10">
+        <v>1.76455473899841</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>20</v>
+      </c>
+      <c r="C14">
+        <v>20</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>7.52235531806945</v>
+      </c>
+      <c r="F14">
+        <v>9.9651515483856201E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>20</v>
+      </c>
+      <c r="C15">
+        <v>20</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>2.03090095520019</v>
+      </c>
+      <c r="F15">
+        <v>119.672306060791</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <v>20</v>
+      </c>
+      <c r="C16">
+        <v>20</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>2.0150196552276598</v>
+      </c>
+      <c r="F16">
+        <v>240.92734432220399</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17">
+        <v>8</v>
+      </c>
+      <c r="B17">
+        <v>20</v>
+      </c>
+      <c r="C17">
+        <v>20</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>2.0048916339874201</v>
+      </c>
+      <c r="F17">
+        <v>491.96847343444801</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>19</v>
+      </c>
+      <c r="C18">
+        <v>20</v>
+      </c>
+      <c r="D18">
+        <v>0.95</v>
+      </c>
+      <c r="E18">
+        <v>2.0036807060241699</v>
+      </c>
+      <c r="F18">
+        <v>1013.6589012145899</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19">
+        <v>32</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>20</v>
+      </c>
+      <c r="D19">
+        <v>0.9</v>
+      </c>
+      <c r="E19">
+        <v>2.0042469501495299</v>
+      </c>
+      <c r="F19">
+        <v>2207.9646835327098</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20">
+        <v>64</v>
+      </c>
+      <c r="B20">
+        <v>16</v>
+      </c>
+      <c r="C20">
+        <v>20</v>
+      </c>
+      <c r="D20">
+        <v>0.8</v>
+      </c>
+      <c r="E20">
+        <v>2.0304780006408598</v>
+      </c>
+      <c r="F20">
+        <v>5181.68605041503</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21">
+        <v>128</v>
+      </c>
+      <c r="B21">
+        <v>7</v>
+      </c>
+      <c r="C21">
+        <v>20</v>
+      </c>
+      <c r="D21">
+        <v>0.35</v>
+      </c>
+      <c r="E21">
+        <v>1.9716362953186</v>
+      </c>
+      <c r="F21">
+        <v>17603.9998779296</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>